<commit_message>
myScaler scales only selected columns
</commit_message>
<xml_diff>
--- a/results/DecisionTreeClassifier-estimator_df.xlsx
+++ b/results/DecisionTreeClassifier-estimator_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,30 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Best Score</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Seed</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Train F1 Weighted </t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">Test F1 Weighted </t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Y Val</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Y Pred</t>
         </is>
@@ -492,22 +497,25 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>0.4365681753771671</v>
+      </c>
+      <c r="E2" t="n">
         <v>42</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.6796636543180321</v>
-      </c>
       <c r="F2" t="n">
-        <v>0.4611594202898551</v>
-      </c>
-      <c r="G2" t="inlineStr">
+        <v>0.6535244922341696</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.5595238095238095</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>[1 0 1 0 0 1 1 1 1 1 1 1 1 0 1 0 0 0 1 0 1 1 0 0]</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>[0 1 0 1 0 0 1 1 0 1 0 1 0 0 1 0 1 0 1 0 0 0 1 1]</t>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>[0 0 0 0 0 0 0 1 0 1 0 1 1 0 1 0 0 0 0 0 0 0 0 1]</t>
         </is>
       </c>
     </row>
@@ -533,22 +541,25 @@
         </is>
       </c>
       <c r="D3" t="n">
+        <v>0.4102855230574304</v>
+      </c>
+      <c r="E3" t="n">
         <v>69</v>
       </c>
-      <c r="E3" t="n">
-        <v>0.6361857825567503</v>
-      </c>
       <c r="F3" t="n">
-        <v>0.5862470862470862</v>
-      </c>
-      <c r="G3" t="inlineStr">
+        <v>0.643601559730592</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.5370370370370371</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>[0 1 1 0 1 0 0 0 1 1 1 0 1 0 1 0 1 0 1 1 0 1 1 1]</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>[1 1 1 0 0 1 0 0 1 0 1 0 1 1 0 0 1 0 1 0 1 0 1 0]</t>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>[0 1 1 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0]</t>
         </is>
       </c>
     </row>
@@ -574,22 +585,25 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>0.4027467843474035</v>
+      </c>
+      <c r="E4" t="n">
         <v>23</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.6583078979392343</v>
-      </c>
       <c r="F4" t="n">
-        <v>0.4611992945326279</v>
-      </c>
-      <c r="G4" t="inlineStr">
+        <v>0.6120975202172421</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>[0 0 1 0 0 1 0 1 1 1 1 1 1 1 1 0 0 0 1 0 1 1 1 0]</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>[0 0 1 1 1 0 1 0 0 1 1 0 0 1 0 0 1 1 1 0 1 1 0 1]</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>[0 1 1 0 0 0 1 1 1 0 0 1 1 0 0 0 1 0 0 1 1 0 0 0]</t>
         </is>
       </c>
     </row>
@@ -615,22 +629,25 @@
         </is>
       </c>
       <c r="D5" t="n">
+        <v>0.5359614936745103</v>
+      </c>
+      <c r="E5" t="n">
         <v>99</v>
       </c>
-      <c r="E5" t="n">
-        <v>0.6999969365560763</v>
-      </c>
       <c r="F5" t="n">
-        <v>0.337995337995338</v>
-      </c>
-      <c r="G5" t="inlineStr">
+        <v>0.6363079373832061</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.4140955837870539</v>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>[0 0 1 1 0 1 1 1 1 0 1 1 0 1 1 0 0 1 0 1 1 0 0 1]</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>[1 0 1 0 1 0 0 0 1 1 0 0 1 1 0 0 1 1 0 0 0 1 1 1]</t>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>[0 0 1 0 0 0 1 0 0 1 0 0 1 0 1 0 0 0 0 0 0 0 0 0]</t>
         </is>
       </c>
     </row>
@@ -656,22 +673,25 @@
         </is>
       </c>
       <c r="D6" t="n">
+        <v>0.4832580875773095</v>
+      </c>
+      <c r="E6" t="n">
         <v>89</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.7090496948561464</v>
-      </c>
       <c r="F6" t="n">
-        <v>0.4888888888888889</v>
-      </c>
-      <c r="G6" t="inlineStr">
+        <v>0.7227056764191048</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>[1 0 1 0 1 1 0 0 1 1 0 1 0 1 1 1 1 1 0 1 0 0 1 0]</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>[1 0 1 1 1 0 1 1 1 0 1 1 0 1 1 0 1 0 1 1 0 1 0 1]</t>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>[0 0 0 1 1 0 0 0 0 1 0 1 0 0 0 1 0 0 1 1 1 0 1 1]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
scaling certain cols works with Decision Tree, gives better results
</commit_message>
<xml_diff>
--- a/results/DecisionTreeClassifier-estimator_df.xlsx
+++ b/results/DecisionTreeClassifier-estimator_df.xlsx
@@ -481,7 +481,26 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()),
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('StandardScaler',
+                                                  StandardScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta_PV',
+                                                   'Delta_RT', 'FullPath_HR',
+                                                   'FullPath_V', 'MT_HR',
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  DecisionTreeClassifier(class_weight='balanced', max_depth=4,
@@ -493,20 +512,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('StandardScaler', StandardScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.4365681753771671</v>
+        <v>0.5387144812980054</v>
       </c>
       <c r="E2" t="n">
         <v>42</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6535244922341696</v>
+        <v>0.7121122738459804</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5595238095238095</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -515,7 +544,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[0 0 0 0 0 0 0 1 0 1 0 1 1 0 1 0 0 0 0 0 0 0 0 1]</t>
+          <t>[0 1 1 1 1 0 1 1 0 1 1 1 1 0 1 0 0 0 1 0 0 0 1 1]</t>
         </is>
       </c>
     </row>
@@ -525,7 +554,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()),
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('StandardScaler',
+                                                  StandardScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta_PV',
+                                                   'Delta_RT', 'FullPath_HR',
+                                                   'FullPath_V', 'MT_HR',
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  DecisionTreeClassifier(class_weight='balanced', max_depth=4,
@@ -537,20 +585,30 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('StandardScaler', StandardScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.4102855230574304</v>
+        <v>0.5236397472795373</v>
       </c>
       <c r="E3" t="n">
         <v>69</v>
       </c>
       <c r="F3" t="n">
-        <v>0.643601559730592</v>
+        <v>0.7275612534486958</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5370370370370371</v>
+        <v>0.6967109424414927</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -559,7 +617,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[0 1 1 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0]</t>
+          <t>[1 1 1 0 1 1 1 0 0 1 0 0 1 0 1 0 1 1 1 1 1 1 1 1]</t>
         </is>
       </c>
     </row>
@@ -569,7 +627,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()),
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('StandardScaler',
+                                                  StandardScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta_PV',
+                                                   'Delta_RT', 'FullPath_HR',
+                                                   'FullPath_V', 'MT_HR',
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  DecisionTreeClassifier(class_weight='balanced', max_depth=4,
@@ -581,20 +658,30 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('StandardScaler', StandardScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.4027467843474035</v>
+        <v>0.4535291717077287</v>
       </c>
       <c r="E4" t="n">
         <v>23</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6120975202172421</v>
+        <v>0.6819285466527922</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -603,7 +690,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[0 1 1 0 0 0 1 1 1 0 0 1 1 0 0 0 1 0 0 1 1 0 0 0]</t>
+          <t>[0 1 1 1 0 1 1 1 1 1 1 1 0 1 1 1 0 0 1 1 1 1 0 1]</t>
         </is>
       </c>
     </row>
@@ -613,7 +700,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()),
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('StandardScaler',
+                                                  StandardScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta_PV',
+                                                   'Delta_RT', 'FullPath_HR',
+                                                   'FullPath_V', 'MT_HR',
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  DecisionTreeClassifier(class_weight='balanced', max_depth=4,
@@ -625,20 +731,30 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('StandardScaler', StandardScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.5359614936745103</v>
+        <v>0.5797953697937545</v>
       </c>
       <c r="E5" t="n">
         <v>99</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6363079373832061</v>
+        <v>0.7435179549604384</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4140955837870539</v>
+        <v>0.4207459207459207</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -647,7 +763,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[0 0 1 0 0 0 1 0 0 1 0 0 1 0 1 0 0 0 0 0 0 0 0 0]</t>
+          <t>[0 0 1 1 1 0 0 0 0 1 0 1 1 0 0 1 1 1 1 0 1 0 0 1]</t>
         </is>
       </c>
     </row>
@@ -657,7 +773,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pipeline(steps=[('scaler', StandardScaler()),
+          <t>Pipeline(steps=[('scaler',
+                 ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                                   transformers=[('StandardScaler',
+                                                  StandardScaler(),
+                                                  ['AE_HR', 'AE_V',
+                                                   'AbsOffAxis_HR',
+                                                   'AbsOffAxis_V',
+                                                   'AbsOnAxis_HR',
+                                                   'AbsOnAxis_V', 'BallPath_HR',
+                                                   'BallPath_V', 'CMT_HR',
+                                                   'CMT_V', 'Corrective_HR',
+                                                   'Corrective_V', 'Delta_AE',
+                                                   'Delta_Fullpath', 'Delta_MT',
+                                                   'Delta_OffAxis',
+                                                   'Delta_OnAxis', 'Delta_PV',
+                                                   'Delta_RT', 'FullPath_HR',
+                                                   'FullPath_V', 'MT_HR',
+                                                   'MT_V', 'PeakV_HR',
+                                                   'PeakV_V', 'RT_HR', 'RT_V',
+                                                   'TMT_HR', 'TMT_V', 'VE_HR', ...])])),
                 ('selector', RandomUnderSampler(random_state=42)),
                 ('model',
                  DecisionTreeClassifier(class_weight='balanced', max_depth=4,
@@ -669,20 +804,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': StandardScaler(), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
+          <t>{'selector': RandomUnderSampler(random_state=42), 'scaler': ColumnTransformer(n_jobs=-1, remainder='passthrough',
+                  transformers=[('StandardScaler', StandardScaler(),
+                                 ['AE_HR', 'AE_V', 'AbsOffAxis_HR',
+                                  'AbsOffAxis_V', 'AbsOnAxis_HR', 'AbsOnAxis_V',
+                                  'BallPath_HR', 'BallPath_V', 'CMT_HR',
+                                  'CMT_V', 'Corrective_HR', 'Corrective_V',
+                                  'Delta_AE', 'Delta_Fullpath', 'Delta_MT',
+                                  'Delta_OffAxis', 'Delta_OnAxis', 'Delta_PV',
+                                  'Delta_RT', 'FullPath_HR', 'FullPath_V',
+                                  'MT_HR', 'MT_V', 'PeakV_HR', 'PeakV_V',
+                                  'RT_HR', 'RT_V', 'TMT_HR', 'TMT_V', 'VE_HR', ...])]), 'model__min_samples_split': 13, 'model__min_samples_leaf': 11, 'model__max_features': 'sqrt', 'model__max_depth': 4, 'model__criterion': 'gini', 'model__class_weight': 'balanced'}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.4832580875773095</v>
+        <v>0.5230189578658997</v>
       </c>
       <c r="E6" t="n">
         <v>89</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7227056764191048</v>
+        <v>0.7013753438359589</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -691,7 +836,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>[0 0 0 1 1 0 0 0 0 1 0 1 0 0 0 1 0 0 1 1 1 0 1 1]</t>
+          <t>[0 0 1 1 1 0 0 0 1 1 1 1 0 1 1 1 0 0 0 1 0 1 1 1]</t>
         </is>
       </c>
     </row>

</xml_diff>